<commit_message>
Definicion de Plan de Entrenamiento y comentarios de los demas numerales.
</commit_message>
<xml_diff>
--- a/SOFTWARE PROJECT MANAGEMENT PLANTS.xlsx
+++ b/SOFTWARE PROJECT MANAGEMENT PLANTS.xlsx
@@ -279,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,12 +313,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -399,21 +393,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,11 +727,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="4" t="s">
         <v>59</v>
       </c>
@@ -803,33 +793,33 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -840,12 +830,12 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>68</v>
       </c>
       <c r="H13" t="s">
@@ -856,12 +846,12 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="21" t="s">
         <v>69</v>
       </c>
       <c r="H14" t="s">
@@ -869,10 +859,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="F15" s="14" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="F15" s="13" t="s">
         <v>70</v>
       </c>
       <c r="H15" t="s">
@@ -883,42 +873,42 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="11"/>
       <c r="F16" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="F17" s="18" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="F17" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="5">
         <v>11.1</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="5">
         <v>11.1</v>
       </c>
@@ -927,357 +917,357 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="22" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="11" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="15" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="11"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="15" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="15" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="15" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="19" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="13" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="13" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="25" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="13" t="s">
+      <c r="A49" s="11"/>
+      <c r="B49" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="11"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="16" t="s">
+      <c r="A50" s="11"/>
+      <c r="B50" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="12"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="13" t="s">
+      <c r="A51" s="11"/>
+      <c r="B51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="11"/>
+      <c r="B52" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="12"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="5">
         <v>11.1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="11"/>
+      <c r="B57" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="11"/>
+      <c r="B58" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="12"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="25" t="s">
+      <c r="A59" s="11"/>
+      <c r="B59" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="12"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="11" t="s">
+      <c r="A60" s="11"/>
+      <c r="B60" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="11"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12" t="s">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="12"/>
+      <c r="C61" s="11"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="11" t="s">
+      <c r="A62" s="11"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="23" t="s">
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="16" t="s">
+      <c r="A64" s="11"/>
+      <c r="B64" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="13"/>
+      <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15" t="s">
+      <c r="A65" s="11"/>
+      <c r="B65" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="13"/>
+      <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="11" t="s">
+      <c r="A66" s="11"/>
+      <c r="B66" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="13"/>
+      <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="16" t="s">
+      <c r="A67" s="11"/>
+      <c r="B67" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="13"/>
+      <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="5">
         <v>11.1</v>
       </c>
@@ -1286,7 +1276,7 @@
       <c r="A70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D71" s="5">

</xml_diff>